<commit_message>
added collapsible feature for current and old chapters in course
</commit_message>
<xml_diff>
--- a/app/assets/data/QuizQuestions.xlsx
+++ b/app/assets/data/QuizQuestions.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26009"/>
-  <workbookPr showInkAnnotation="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/SrinjoyMajumdar/Documents/AtsaCorp/ImagineDragons/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="4720" windowWidth="27760" windowHeight="16240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t xml:space="preserve">Test Question 1 </t>
   </si>
@@ -51,6 +46,18 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>Question1.jpg</t>
+  </si>
+  <si>
+    <t>Question2.jpg</t>
+  </si>
+  <si>
+    <t>Question3.jpg</t>
+  </si>
+  <si>
+    <t>What planet is this?</t>
   </si>
 </sst>
 </file>
@@ -86,8 +93,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,7 +153,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -180,7 +188,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,7 +365,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -365,15 +373,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1">
         <v>1</v>
       </c>
@@ -381,13 +392,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>2</v>
       </c>
@@ -400,8 +414,11 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>3</v>
       </c>
@@ -414,8 +431,11 @@
       <c r="D3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>4</v>
       </c>
@@ -429,7 +449,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>5</v>
       </c>
@@ -443,7 +463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>6</v>
       </c>
@@ -457,7 +477,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>7</v>
       </c>
@@ -471,7 +491,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>8</v>
       </c>
@@ -485,7 +505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>9</v>
       </c>
@@ -499,7 +519,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>10</v>
       </c>
@@ -513,7 +533,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>11</v>
       </c>
@@ -527,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>12</v>
       </c>
@@ -541,7 +561,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>13</v>
       </c>
@@ -555,7 +575,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>14</v>
       </c>
@@ -569,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>15</v>
       </c>
@@ -583,7 +603,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>16</v>
       </c>
@@ -597,7 +617,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>17</v>
       </c>
@@ -611,7 +631,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>18</v>
       </c>
@@ -625,7 +645,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>19</v>
       </c>
@@ -639,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>20</v>
       </c>
@@ -655,5 +675,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>